<commit_message>
Oppdaterte Nina med sluttspill
</commit_message>
<xml_diff>
--- a/PredictionSheets/VM 2014 Tippekonkuranse - Nina.xlsx
+++ b/PredictionSheets/VM 2014 Tippekonkuranse - Nina.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nina.h.brattetaule\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppespilltipp" sheetId="1" r:id="rId1"/>
     <sheet name="Sluttspilltipp" sheetId="2" r:id="rId2"/>
     <sheet name="Kampoppsett" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="136">
   <si>
     <t>Group A</t>
   </si>
@@ -164,54 +169,6 @@
     <t>Sluttspill</t>
   </si>
   <si>
-    <t>Vinner Gruppe B</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe C</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe C</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe A</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe A</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe B</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe D</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe D</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe E</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe E</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe F</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe F</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe G</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe G</t>
-  </si>
-  <si>
-    <t>Vinner Gruppe H</t>
-  </si>
-  <si>
-    <t>Andreplass Gruppe H</t>
-  </si>
-  <si>
     <t>Lag i kvartfinaler:</t>
   </si>
   <si>
@@ -221,18 +178,6 @@
     <t>Sluttstilling topp 4:</t>
   </si>
   <si>
-    <t>Gull</t>
-  </si>
-  <si>
-    <t>Sølv</t>
-  </si>
-  <si>
-    <t>Bronse</t>
-  </si>
-  <si>
-    <t>Fjerdeplass</t>
-  </si>
-  <si>
     <t>Lag i åttendedelsfinaler:</t>
   </si>
   <si>
@@ -474,17 +419,32 @@
   </si>
   <si>
     <t>Nina</t>
+  </si>
+  <si>
+    <t>Nederland</t>
+  </si>
+  <si>
+    <t>Spania</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Frankrike</t>
+  </si>
+  <si>
+    <t>Hinduras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-414]d/\ mmmm;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1544,7 +1504,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1586,7 +1546,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1618,9 +1578,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1652,6 +1613,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1827,23 +1789,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>44</v>
       </c>
@@ -1853,18 +1815,18 @@
       <c r="N1" s="64"/>
       <c r="O1" s="64"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L2" s="64"/>
       <c r="M2" s="64"/>
       <c r="N2" s="64"/>
       <c r="O2" s="64"/>
     </row>
-    <row r="3" spans="1:15" ht="27.95" customHeight="1" thickBot="1">
+    <row r="3" spans="1:15" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -1874,13 +1836,13 @@
       <c r="N3" s="64"/>
       <c r="O3" s="64"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L4" s="64"/>
       <c r="M4" s="64"/>
       <c r="N4" s="64"/>
       <c r="O4" s="64"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1898,7 +1860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1913,7 +1875,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1939,22 +1901,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="27.95" customHeight="1">
+    <row r="11" spans="1:15" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="4">
-        <v>2</v>
-      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="4">
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>122</v>
-      </c>
+      <c r="E11" s="12"/>
       <c r="G11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1972,7 +1930,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="27.95" customHeight="1">
+    <row r="12" spans="1:15" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>3</v>
       </c>
@@ -1985,9 +1943,7 @@
       <c r="D12" s="3">
         <v>2</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>94</v>
-      </c>
+      <c r="E12" s="13"/>
       <c r="G12" s="8" t="s">
         <v>23</v>
       </c>
@@ -2005,7 +1961,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="27.95" customHeight="1">
+    <row r="13" spans="1:15" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>1</v>
       </c>
@@ -2039,7 +1995,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="27.95" customHeight="1">
+    <row r="14" spans="1:15" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>4</v>
       </c>
@@ -2073,7 +2029,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="27.95" customHeight="1">
+    <row r="15" spans="1:15" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -2107,7 +2063,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="27.95" customHeight="1" thickBot="1">
+    <row r="16" spans="1:15" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
@@ -2141,7 +2097,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20.25" customHeight="1">
+    <row r="17" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
@@ -2149,7 +2105,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
+    <row r="18" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -2163,7 +2119,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="27.95" customHeight="1">
+    <row r="19" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
@@ -2197,7 +2153,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="27.95" customHeight="1">
+    <row r="20" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>8</v>
       </c>
@@ -2231,7 +2187,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27.95" customHeight="1">
+    <row r="21" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2221,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="27.95" customHeight="1">
+    <row r="22" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>9</v>
       </c>
@@ -2299,7 +2255,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27.95" customHeight="1">
+    <row r="23" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>9</v>
       </c>
@@ -2333,7 +2289,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="27.95" customHeight="1" thickBot="1">
+    <row r="24" spans="1:11" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
@@ -2367,7 +2323,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20.25" customHeight="1">
+    <row r="25" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
@@ -2375,7 +2331,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
+    <row r="26" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2389,7 +2345,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="27.95" customHeight="1">
+    <row r="27" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
@@ -2423,7 +2379,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="27.95" customHeight="1">
+    <row r="28" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>13</v>
       </c>
@@ -2457,7 +2413,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="27.95" customHeight="1">
+    <row r="29" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -2491,7 +2447,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="27.95" customHeight="1">
+    <row r="30" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>14</v>
       </c>
@@ -2525,7 +2481,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="27.95" customHeight="1">
+    <row r="31" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
@@ -2559,7 +2515,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="27.95" customHeight="1" thickBot="1">
+    <row r="32" spans="1:11" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>12</v>
       </c>
@@ -2593,7 +2549,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="20.25" customHeight="1">
+    <row r="33" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="2"/>
@@ -2601,7 +2557,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="20.25" customHeight="1" thickBot="1">
+    <row r="34" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2615,7 +2571,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="27.95" customHeight="1">
+    <row r="35" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>16</v>
       </c>
@@ -2649,7 +2605,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="27.95" customHeight="1">
+    <row r="36" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>18</v>
       </c>
@@ -2683,7 +2639,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="27.95" customHeight="1">
+    <row r="37" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>16</v>
       </c>
@@ -2717,7 +2673,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="27.95" customHeight="1">
+    <row r="38" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>19</v>
       </c>
@@ -2751,7 +2707,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="27.95" customHeight="1">
+    <row r="39" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>19</v>
       </c>
@@ -2785,7 +2741,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="27.95" customHeight="1" thickBot="1">
+    <row r="40" spans="1:11" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>17</v>
       </c>
@@ -2819,7 +2775,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
     </row>
   </sheetData>
@@ -2835,17 +2791,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet2">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -2853,120 +2809,144 @@
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="24" customHeight="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A7" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A10" s="31" t="s">
-        <v>63</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
     </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-    </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A12" s="36"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="24" customHeight="1" thickBot="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="42" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2981,8 +2961,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2992,7 +2972,7 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
@@ -3000,41 +2980,41 @@
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="50">
         <v>41802</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D2" s="53">
         <v>0.91666666666666663</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="G2" s="48"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="54">
         <v>41803</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D3" s="56">
         <v>0.75</v>
@@ -3046,22 +3026,22 @@
         <v>49</v>
       </c>
       <c r="H3" s="71" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I3" s="71"/>
       <c r="J3" s="72">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="54">
         <v>41807</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D4" s="56">
         <v>0.875</v>
@@ -3073,22 +3053,22 @@
         <v>50</v>
       </c>
       <c r="H4" s="75" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="I4" s="75"/>
       <c r="J4" s="76">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="54">
         <v>41809</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D5" s="56">
         <v>1</v>
@@ -3100,22 +3080,22 @@
         <v>51</v>
       </c>
       <c r="H5" s="75" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="I5" s="75"/>
       <c r="J5" s="76">
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="54">
         <v>41813</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D6" s="56">
         <v>0.91666666666666663</v>
@@ -3127,22 +3107,22 @@
         <v>52</v>
       </c>
       <c r="H6" s="75" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="I6" s="75"/>
       <c r="J6" s="76">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="57">
         <v>41813</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D7" s="60">
         <v>0.91666666666666663</v>
@@ -3154,14 +3134,14 @@
         <v>53</v>
       </c>
       <c r="H7" s="75" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="I7" s="75"/>
       <c r="J7" s="76">
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="61"/>
       <c r="B8" s="62"/>
       <c r="C8" s="21"/>
@@ -3173,22 +3153,22 @@
         <v>54</v>
       </c>
       <c r="H8" s="75" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="I8" s="75"/>
       <c r="J8" s="76">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="50">
         <v>41803</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D9" s="53">
         <v>0.875</v>
@@ -3200,22 +3180,22 @@
         <v>55</v>
       </c>
       <c r="H9" s="75" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="I9" s="75"/>
       <c r="J9" s="76">
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="54">
         <v>41804</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D10" s="56">
         <v>1</v>
@@ -3227,22 +3207,22 @@
         <v>56</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="I10" s="79"/>
       <c r="J10" s="80">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="54">
         <v>41808</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D11" s="56">
         <v>0.75</v>
@@ -3250,33 +3230,33 @@
       <c r="F11" s="46"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="54">
         <v>41808</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D12" s="56">
         <v>0.875</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="54">
         <v>41813</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D13" s="56">
         <v>0.75</v>
@@ -3288,22 +3268,22 @@
         <v>57</v>
       </c>
       <c r="H13" s="71" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="I13" s="71"/>
       <c r="J13" s="72">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="57">
         <v>41813</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C14" s="59" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D14" s="60">
         <v>0.75</v>
@@ -3315,14 +3295,14 @@
         <v>58</v>
       </c>
       <c r="H14" s="75" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="I14" s="75"/>
       <c r="J14" s="76">
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="64" customFormat="1">
+    <row r="15" spans="1:11" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="61"/>
       <c r="B15" s="62"/>
       <c r="C15" s="21"/>
@@ -3334,22 +3314,22 @@
         <v>59</v>
       </c>
       <c r="H15" s="75" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="I15" s="75"/>
       <c r="J15" s="76">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
         <v>41804</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D16" s="53">
         <v>0.75</v>
@@ -3362,7 +3342,7 @@
         <v>60</v>
       </c>
       <c r="H16" s="79" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="I16" s="79"/>
       <c r="J16" s="80">
@@ -3370,15 +3350,15 @@
       </c>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="54">
         <v>41805</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D17" s="56">
         <v>0.125</v>
@@ -3386,33 +3366,33 @@
       <c r="F17" s="46"/>
       <c r="G17" s="49"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="54">
         <v>41809</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D18" s="56">
         <v>0.75</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="G18" s="49"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="54">
         <v>41810</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D19" s="56">
         <v>1</v>
@@ -3424,22 +3404,22 @@
         <v>61</v>
       </c>
       <c r="H19" s="71" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="I19" s="71"/>
       <c r="J19" s="72">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="54">
         <v>41814</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D20" s="56">
         <v>0.91666666666666663</v>
@@ -3451,22 +3431,22 @@
         <v>62</v>
       </c>
       <c r="H20" s="79" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="I20" s="79"/>
       <c r="J20" s="80">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="57">
         <v>41814</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C21" s="59" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D21" s="60">
         <v>0.91666666666666663</v>
@@ -3474,25 +3454,25 @@
       <c r="F21" s="46"/>
       <c r="G21" s="49"/>
     </row>
-    <row r="22" spans="1:10" s="64" customFormat="1">
+    <row r="22" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="61"/>
       <c r="B22" s="62"/>
       <c r="C22" s="21"/>
       <c r="D22" s="63"/>
       <c r="F22" s="65" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="G22" s="66"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
         <v>41804</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="D23" s="53">
         <v>0.875</v>
@@ -3502,22 +3482,22 @@
       </c>
       <c r="G23" s="82"/>
       <c r="H23" s="83" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="I23" s="83"/>
       <c r="J23" s="84">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="54">
         <v>41805</v>
       </c>
       <c r="B24" s="55" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="D24" s="56">
         <v>1</v>
@@ -3525,33 +3505,33 @@
       <c r="F24" s="46"/>
       <c r="G24" s="49"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="54">
         <v>41809</v>
       </c>
       <c r="B25" s="55" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="D25" s="56">
         <v>0.75</v>
       </c>
       <c r="F25" s="46" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="G25" s="49"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="54">
         <v>41810</v>
       </c>
       <c r="B26" s="55" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D26" s="56">
         <v>0.875</v>
@@ -3561,44 +3541,44 @@
       </c>
       <c r="G26" s="82"/>
       <c r="H26" s="83" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="I26" s="83"/>
       <c r="J26" s="84">
         <v>0.875</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="54">
         <v>41814</v>
       </c>
       <c r="B27" s="55" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D27" s="56">
         <v>0.75</v>
       </c>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="57">
         <v>41814</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C28" s="59" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D28" s="60">
         <v>0.75</v>
       </c>
       <c r="F28" s="45"/>
     </row>
-    <row r="29" spans="1:10" s="64" customFormat="1">
+    <row r="29" spans="1:10" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="62"/>
       <c r="C29" s="21"/>
@@ -3606,15 +3586,15 @@
       <c r="F29" s="67"/>
       <c r="G29" s="68"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
         <v>41805</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D30" s="53">
         <v>0.75</v>
@@ -3624,349 +3604,349 @@
       <c r="G30" s="86"/>
       <c r="H30" s="87"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="54">
         <v>41805</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D31" s="56">
         <v>0.875</v>
       </c>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="54">
         <v>41810</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D32" s="56">
         <v>0.875</v>
       </c>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="54">
         <v>41811</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D33" s="56">
         <v>1</v>
       </c>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="54">
         <v>41815</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D34" s="56">
         <v>0.91666666666666663</v>
       </c>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="57">
         <v>41815</v>
       </c>
       <c r="B35" s="58" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C35" s="59" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D35" s="60">
         <v>0.91666666666666663</v>
       </c>
       <c r="F35" s="45"/>
     </row>
-    <row r="36" spans="1:7" s="64" customFormat="1">
+    <row r="36" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="61"/>
       <c r="B36" s="62"/>
       <c r="C36" s="21"/>
       <c r="D36" s="63"/>
       <c r="G36" s="68"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
         <v>41806</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="D37" s="53">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="54">
         <v>41806</v>
       </c>
       <c r="B38" s="55" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D38" s="56">
         <v>0.875</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="54">
         <v>41811</v>
       </c>
       <c r="B39" s="55" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D39" s="56">
         <v>0.75</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="54">
         <v>41812</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D40" s="56">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="54">
         <v>41815</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="D41" s="56">
         <v>0.75</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="57">
         <v>41815</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C42" s="59" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D42" s="60">
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="64" customFormat="1">
+    <row r="43" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="61"/>
       <c r="B43" s="62"/>
       <c r="C43" s="21"/>
       <c r="D43" s="63"/>
       <c r="G43" s="68"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
         <v>41806</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D44" s="53">
         <v>0.75</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="54">
         <v>41807</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="D45" s="56">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="54">
         <v>41811</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="D46" s="56">
         <v>0.875</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="54">
         <v>41813</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D47" s="56">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="54">
         <v>41816</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D48" s="56">
         <v>0.75</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="57">
         <v>41816</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C49" s="59" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="D49" s="60">
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="64" customFormat="1">
+    <row r="50" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="61"/>
       <c r="B50" s="62"/>
       <c r="C50" s="21"/>
       <c r="D50" s="63"/>
       <c r="G50" s="68"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <v>41807</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="D51" s="53">
         <v>0.75</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="54">
         <v>41808</v>
       </c>
       <c r="B52" s="55" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D52" s="56">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="54">
         <v>41812</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="D53" s="56">
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="54">
         <v>41812</v>
       </c>
       <c r="B54" s="55" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D54" s="56">
         <v>0.875</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="54">
         <v>41816</v>
       </c>
       <c r="B55" s="55" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="D55" s="56">
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="57">
         <v>41816</v>
       </c>
       <c r="B56" s="58" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C56" s="59" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D56" s="60">
         <v>0.91666666666666663</v>

</xml_diff>